<commit_message>
koordinatat e pikave edit zona
</commit_message>
<xml_diff>
--- a/cd/7---Koordinatat-e-pikave-për-parcelë.xlsx
+++ b/cd/7---Koordinatat-e-pikave-për-parcelë.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
   <si>
     <t>Nr</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>3583-7</t>
+  </si>
+  <si>
+    <t>SEAD PRUSHI</t>
   </si>
 </sst>
 </file>
@@ -832,120 +835,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -957,6 +846,120 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1153,7 +1156,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>Zona Kadastrale: Talinoc i Jerlive</a:t>
+            <a:t>Zona Kadastrale: Jezerc</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1228,7 +1231,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>: 00231-0</a:t>
+            <a:t>: 03583-2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1598,13 +1601,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
@@ -1614,106 +1617,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89"/>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="A1" s="109"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
     </row>
     <row r="2" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
+      <c r="A2" s="109"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="88"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
+      <c r="A4" s="108"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="108"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
+      <c r="A5" s="108"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
+      <c r="A6" s="108"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="81"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="101"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="82"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="84"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="104"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="85"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="87"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="106"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="107"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
@@ -1878,25 +1881,25 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="114">
+      <c r="C21" s="76">
         <v>1</v>
       </c>
-      <c r="D21" s="115">
+      <c r="D21" s="77">
         <v>7501824.8183000004</v>
       </c>
-      <c r="E21" s="115">
+      <c r="E21" s="77">
         <v>4691763.1796000004</v>
       </c>
-      <c r="F21" s="116">
+      <c r="F21" s="78">
         <v>820.32</v>
       </c>
-      <c r="G21" s="117">
+      <c r="G21" s="79">
         <v>2</v>
       </c>
-      <c r="H21" s="118" t="s">
+      <c r="H21" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="119" t="s">
+      <c r="I21" s="81" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1907,17 +1910,17 @@
       <c r="A23" s="5"/>
     </row>
     <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="76" t="s">
+      <c r="A24" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="78"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="90"/>
     </row>
     <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -1935,7 +1938,7 @@
       <c r="E25" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="90"/>
+      <c r="F25" s="110"/>
       <c r="G25" s="8" t="s">
         <v>14</v>
       </c>
@@ -1962,16 +1965,16 @@
       <c r="E26" s="12">
         <v>820.3075</v>
       </c>
-      <c r="F26" s="91"/>
-      <c r="G26" s="74">
+      <c r="F26" s="111"/>
+      <c r="G26" s="97">
         <f>C26-C27</f>
         <v>-6.9000003859400749E-3</v>
       </c>
-      <c r="H26" s="74">
+      <c r="H26" s="97">
         <f>D26-D27</f>
         <v>-1.4999993145465851E-3</v>
       </c>
-      <c r="I26" s="94">
+      <c r="I26" s="114">
         <f>SQRT(G26^2+H26^2)</f>
         <v>7.0611616090848258E-3</v>
       </c>
@@ -1992,10 +1995,10 @@
       <c r="E27" s="12">
         <v>820.33169999999996</v>
       </c>
-      <c r="F27" s="91"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="93"/>
-      <c r="I27" s="96"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="113"/>
+      <c r="I27" s="116"/>
     </row>
     <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
@@ -2013,16 +2016,16 @@
       <c r="E28" s="16">
         <v>814.26589999999999</v>
       </c>
-      <c r="F28" s="91"/>
-      <c r="G28" s="74">
+      <c r="F28" s="111"/>
+      <c r="G28" s="97">
         <f>C28-C29</f>
         <v>1.3399999588727951E-2</v>
       </c>
-      <c r="H28" s="74">
+      <c r="H28" s="97">
         <f>D28-D29</f>
         <v>5.4000001400709152E-3</v>
       </c>
-      <c r="I28" s="94">
+      <c r="I28" s="114">
         <f>SQRT(G28^2+H28^2)</f>
         <v>1.4447144717579151E-2</v>
       </c>
@@ -2043,10 +2046,10 @@
       <c r="E29" s="20">
         <v>814.30619999999999</v>
       </c>
-      <c r="F29" s="92"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="95"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="115"/>
     </row>
     <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
@@ -2095,12 +2098,12 @@
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="76" t="s">
+      <c r="E38" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="77"/>
-      <c r="G38" s="77"/>
-      <c r="H38" s="78"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="90"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
@@ -2273,28 +2276,32 @@
       <c r="B50" s="27"/>
       <c r="C50" s="27"/>
       <c r="D50" s="27"/>
-      <c r="E50" s="103"/>
-      <c r="F50" s="103"/>
-      <c r="G50" s="104"/>
-      <c r="H50" s="97" t="s">
+      <c r="E50" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="F50" s="91"/>
+      <c r="G50" s="92"/>
+      <c r="H50" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="I50" s="98"/>
-      <c r="J50" s="101"/>
+      <c r="I50" s="83"/>
+      <c r="J50" s="86"/>
     </row>
     <row r="51" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="105" t="s">
+      <c r="A51" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="106"/>
-      <c r="C51" s="106"/>
-      <c r="D51" s="106"/>
-      <c r="E51" s="107"/>
-      <c r="F51" s="107"/>
-      <c r="G51" s="108"/>
-      <c r="H51" s="99"/>
-      <c r="I51" s="100"/>
-      <c r="J51" s="102"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="94"/>
+      <c r="D51" s="94"/>
+      <c r="E51" s="95">
+        <v>152</v>
+      </c>
+      <c r="F51" s="95"/>
+      <c r="G51" s="96"/>
+      <c r="H51" s="84"/>
+      <c r="I51" s="85"/>
+      <c r="J51" s="87"/>
     </row>
     <row r="52" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
@@ -2334,12 +2341,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H50:I51"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="E51:G51"/>
     <mergeCell ref="G28:G29"/>
     <mergeCell ref="A24:I24"/>
     <mergeCell ref="C8:I10"/>
@@ -2351,6 +2352,12 @@
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="H28:H29"/>
     <mergeCell ref="H26:H27"/>
+    <mergeCell ref="H50:I51"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="E51:G51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2376,31 +2383,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="G2" s="109" t="s">
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="G2" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
       <c r="O2" s="52"/>
-      <c r="P2" s="110" t="s">
+      <c r="P2" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="54" t="s">
@@ -2461,10 +2468,10 @@
       <c r="W3" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="111" t="s">
+      <c r="X3" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="Y3" s="111"/>
+      <c r="Y3" s="119"/>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="57">
@@ -3143,10 +3150,10 @@
       <c r="W32">
         <v>816.178</v>
       </c>
-      <c r="X32" s="112">
+      <c r="X32" s="74">
         <v>25568</v>
       </c>
-      <c r="Y32" s="113">
+      <c r="Y32" s="75">
         <v>0.66666666666666663</v>
       </c>
       <c r="Z32">
@@ -3185,10 +3192,10 @@
       <c r="W33">
         <v>823.47</v>
       </c>
-      <c r="X33" s="112">
+      <c r="X33" s="74">
         <v>25568</v>
       </c>
-      <c r="Y33" s="113">
+      <c r="Y33" s="75">
         <v>0.66666666666666663</v>
       </c>
       <c r="Z33">
@@ -3226,10 +3233,10 @@
       <c r="W34">
         <v>0</v>
       </c>
-      <c r="X34" s="112">
+      <c r="X34" s="74">
         <v>25568</v>
       </c>
-      <c r="Y34" s="113">
+      <c r="Y34" s="75">
         <v>0.66666666666666663</v>
       </c>
       <c r="Z34">
@@ -3264,10 +3271,10 @@
       <c r="W35">
         <v>819.76400000000001</v>
       </c>
-      <c r="X35" s="112">
+      <c r="X35" s="74">
         <v>44020</v>
       </c>
-      <c r="Y35" s="113">
+      <c r="Y35" s="75">
         <v>0.44290509259259259</v>
       </c>
     </row>
@@ -3299,10 +3306,10 @@
       <c r="W36">
         <v>829.41399999999999</v>
       </c>
-      <c r="X36" s="112">
+      <c r="X36" s="74">
         <v>44020</v>
       </c>
-      <c r="Y36" s="113">
+      <c r="Y36" s="75">
         <v>0.44855324074074071</v>
       </c>
     </row>
@@ -3322,10 +3329,10 @@
       <c r="W37">
         <v>822.95799999999997</v>
       </c>
-      <c r="X37" s="112">
+      <c r="X37" s="74">
         <v>44020</v>
       </c>
-      <c r="Y37" s="113">
+      <c r="Y37" s="75">
         <v>0.45236111111111116</v>
       </c>
     </row>
@@ -3345,10 +3352,10 @@
       <c r="W38">
         <v>817.03700000000003</v>
       </c>
-      <c r="X38" s="112">
+      <c r="X38" s="74">
         <v>44020</v>
       </c>
-      <c r="Y38" s="113">
+      <c r="Y38" s="75">
         <v>0.45324074074074078</v>
       </c>
     </row>

</xml_diff>